<commit_message>
se agregaron las fechas en que se realizaran las actividades hasta el avance 2
</commit_message>
<xml_diff>
--- a/Cronograma Gigis.xlsx
+++ b/Cronograma Gigis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\Semestre10\DAW\Proyecto-Gigi-s\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09344442-EB70-46F5-AC7D-5332BA4D819C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539357A0-27F2-4F37-BB5F-454912F08026}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -130,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t xml:space="preserve"> Period Highlight:</t>
   </si>
@@ -138,9 +138,6 @@
     <t>PERCENT COMPLETE</t>
   </si>
   <si>
-    <t>Select a period to highlight at right.  A legend describing the charting follows.</t>
-  </si>
-  <si>
     <t>&lt; blank &gt;</t>
   </si>
   <si>
@@ -199,9 +196,6 @@
   </si>
   <si>
     <t>MER</t>
-  </si>
-  <si>
-    <t>Prototipo del sistema</t>
   </si>
   <si>
     <t>Acuerdo</t>
@@ -314,6 +308,36 @@
   <si>
     <t>DURACION REAL</t>
   </si>
+  <si>
+    <t>Análisis y diseño de la solucion</t>
+  </si>
+  <si>
+    <t>Reglas de negocio</t>
+  </si>
+  <si>
+    <t>Modelo Entidad-Relación</t>
+  </si>
+  <si>
+    <t>Diccionario de datos</t>
+  </si>
+  <si>
+    <t>Documentación de restricciones</t>
+  </si>
+  <si>
+    <t>Tablas correspondientes (Modelo Relacional)</t>
+  </si>
+  <si>
+    <t>Requisitos no funcionales</t>
+  </si>
+  <si>
+    <t>Mapa del sitio</t>
+  </si>
+  <si>
+    <t>Primera versión de la interfaz de usuario</t>
+  </si>
+  <si>
+    <t>Plan de comunicación</t>
+  </si>
 </sst>
 </file>
 
@@ -322,7 +346,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -513,8 +537,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="20">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -606,12 +638,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -624,7 +650,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -992,18 +1018,12 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1013,9 +1033,6 @@
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="2" applyFont="1" applyFill="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="8" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -1028,9 +1045,6 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="9" xfId="6" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1088,18 +1102,12 @@
     <xf numFmtId="164" fontId="10" fillId="13" borderId="0" xfId="11" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" textRotation="90"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="15" borderId="0" xfId="11" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="90"/>
-    </xf>
     <xf numFmtId="164" fontId="10" fillId="16" borderId="0" xfId="11" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" textRotation="90"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="17" borderId="0" xfId="11" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" textRotation="90"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="18" borderId="0" xfId="11" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1121,12 +1129,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="2" applyFont="1" applyFill="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1136,16 +1138,28 @@
     <xf numFmtId="9" fontId="6" fillId="9" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
@@ -1171,6 +1185,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1192,32 +1209,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="18" borderId="0" xfId="11" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="10" borderId="0" xfId="11" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="9" borderId="0" xfId="11" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1510,6 +1536,72 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>166279</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>186961</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2136532</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>151567</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8D97564-BD95-42DF-9896-9CB02ADEF1AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="166279" y="186961"/>
+          <a:ext cx="3334777" cy="557621"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1741,16 +1833,16 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CI44"/>
+  <dimension ref="A1:CI41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.625" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
     <col min="2" max="2" width="34.5" style="2" customWidth="1"/>
     <col min="3" max="6" width="11.625" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.625" style="4" customWidth="1"/>
@@ -1758,27 +1850,22 @@
     <col min="28" max="87" width="4.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="B1" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="12"/>
+    <row r="1" spans="1:87" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
+      <c r="C1" s="27" t="s">
+        <v>24</v>
+      </c>
       <c r="D1" s="12"/>
-      <c r="E1" s="12">
-        <v>1</v>
-      </c>
+      <c r="E1" s="12"/>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
       <c r="BK1" s="20"/>
     </row>
     <row r="2" spans="1:87" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="76" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
       <c r="G2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1786,161 +1873,161 @@
         <v>1</v>
       </c>
       <c r="J2" s="14"/>
-      <c r="K2" s="98" t="s">
+      <c r="K2" s="79" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="83"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="98" t="s">
+      <c r="R2" s="82"/>
+      <c r="S2" s="82"/>
+      <c r="T2" s="81"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="W2" s="71"/>
+      <c r="X2" s="71"/>
+      <c r="Y2" s="83"/>
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="84" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB2" s="85"/>
+      <c r="AC2" s="85"/>
+      <c r="AD2" s="85"/>
+      <c r="AE2" s="85"/>
+      <c r="AF2" s="85"/>
+      <c r="AG2" s="86"/>
+      <c r="AH2" s="18"/>
+      <c r="AI2" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="R2" s="85"/>
-      <c r="S2" s="85"/>
-      <c r="T2" s="84"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="74" t="s">
-        <v>28</v>
-      </c>
-      <c r="W2" s="75"/>
-      <c r="X2" s="75"/>
-      <c r="Y2" s="86"/>
-      <c r="Z2" s="17"/>
-      <c r="AA2" s="87" t="s">
+      <c r="AJ2" s="71"/>
+      <c r="AK2" s="71"/>
+      <c r="AL2" s="71"/>
+      <c r="AM2" s="71"/>
+      <c r="AN2" s="71"/>
+      <c r="AO2" s="71"/>
+      <c r="AP2" s="71"/>
+      <c r="BK2" s="20"/>
+    </row>
+    <row r="3" spans="1:87" s="52" customFormat="1" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="68"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="68"/>
+      <c r="V3" s="68"/>
+      <c r="W3" s="68"/>
+      <c r="X3" s="68"/>
+      <c r="Y3" s="90"/>
+      <c r="Z3" s="90"/>
+      <c r="AA3" s="90"/>
+      <c r="AB3" s="90"/>
+      <c r="AC3" s="90"/>
+      <c r="AD3" s="90"/>
+      <c r="AE3" s="90"/>
+      <c r="AF3" s="91"/>
+      <c r="AG3" s="91"/>
+      <c r="AH3" s="92"/>
+      <c r="AI3" s="93"/>
+      <c r="AJ3" s="91"/>
+      <c r="AK3" s="91"/>
+      <c r="AL3" s="91"/>
+      <c r="AM3" s="91"/>
+      <c r="AN3" s="91"/>
+      <c r="AO3" s="91"/>
+      <c r="AP3" s="91"/>
+      <c r="AQ3" s="91"/>
+      <c r="AR3" s="91"/>
+      <c r="AS3" s="91"/>
+      <c r="AT3" s="91"/>
+      <c r="AU3" s="91"/>
+      <c r="AV3" s="91"/>
+      <c r="AW3" s="91"/>
+      <c r="AX3" s="91"/>
+      <c r="AY3" s="91"/>
+      <c r="AZ3" s="91"/>
+      <c r="BA3" s="91"/>
+      <c r="BB3" s="91"/>
+      <c r="BC3" s="91"/>
+      <c r="BD3" s="91"/>
+      <c r="BE3" s="91"/>
+      <c r="BF3" s="91"/>
+      <c r="BG3" s="91"/>
+      <c r="BH3" s="91"/>
+      <c r="BI3" s="95"/>
+      <c r="BJ3" s="95"/>
+      <c r="BK3" s="95"/>
+      <c r="BL3" s="95"/>
+      <c r="BM3" s="95"/>
+      <c r="BN3" s="95"/>
+      <c r="BO3" s="95"/>
+      <c r="BP3" s="95"/>
+      <c r="BQ3" s="94"/>
+      <c r="BR3" s="95"/>
+      <c r="BS3" s="95"/>
+      <c r="BT3" s="95"/>
+      <c r="BU3" s="95"/>
+      <c r="BV3" s="95"/>
+      <c r="BW3" s="95"/>
+      <c r="BX3" s="95"/>
+      <c r="BY3" s="95"/>
+      <c r="BZ3" s="95"/>
+      <c r="CA3" s="95"/>
+      <c r="CB3" s="95"/>
+      <c r="CC3" s="95"/>
+      <c r="CD3" s="95"/>
+      <c r="CE3" s="95"/>
+      <c r="CF3" s="95"/>
+      <c r="CG3" s="95"/>
+      <c r="CH3" s="95"/>
+      <c r="CI3" s="95"/>
+    </row>
+    <row r="4" spans="1:87" s="11" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="AB2" s="88"/>
-      <c r="AC2" s="88"/>
-      <c r="AD2" s="88"/>
-      <c r="AE2" s="88"/>
-      <c r="AF2" s="88"/>
-      <c r="AG2" s="89"/>
-      <c r="AH2" s="18"/>
-      <c r="AI2" s="74" t="s">
+      <c r="C4" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="AJ2" s="75"/>
-      <c r="AK2" s="75"/>
-      <c r="AL2" s="75"/>
-      <c r="AM2" s="75"/>
-      <c r="AN2" s="75"/>
-      <c r="AO2" s="75"/>
-      <c r="AP2" s="75"/>
-      <c r="BK2" s="20"/>
-    </row>
-    <row r="3" spans="1:87" s="58" customFormat="1" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="91" t="s">
+      <c r="D4" s="75" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="75" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="75" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="19" t="s">
         <v>11</v>
-      </c>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
-      <c r="P3" s="91"/>
-      <c r="Q3" s="91"/>
-      <c r="R3" s="91"/>
-      <c r="S3" s="91"/>
-      <c r="T3" s="91"/>
-      <c r="U3" s="91"/>
-      <c r="V3" s="91"/>
-      <c r="W3" s="91"/>
-      <c r="X3" s="91"/>
-      <c r="Y3" s="92"/>
-      <c r="Z3" s="92"/>
-      <c r="AA3" s="92"/>
-      <c r="AB3" s="92"/>
-      <c r="AC3" s="92"/>
-      <c r="AD3" s="92"/>
-      <c r="AE3" s="92"/>
-      <c r="AF3" s="92"/>
-      <c r="AG3" s="92"/>
-      <c r="AH3" s="93"/>
-      <c r="AI3" s="94"/>
-      <c r="AJ3" s="95"/>
-      <c r="AK3" s="95"/>
-      <c r="AL3" s="95"/>
-      <c r="AM3" s="95"/>
-      <c r="AN3" s="95"/>
-      <c r="AO3" s="95"/>
-      <c r="AP3" s="95"/>
-      <c r="AQ3" s="95"/>
-      <c r="AR3" s="95"/>
-      <c r="AS3" s="95"/>
-      <c r="AT3" s="95"/>
-      <c r="AU3" s="95"/>
-      <c r="AV3" s="95"/>
-      <c r="AW3" s="95"/>
-      <c r="AX3" s="95"/>
-      <c r="AY3" s="95"/>
-      <c r="AZ3" s="95"/>
-      <c r="BA3" s="95"/>
-      <c r="BB3" s="95"/>
-      <c r="BC3" s="95"/>
-      <c r="BD3" s="95"/>
-      <c r="BE3" s="95"/>
-      <c r="BF3" s="95"/>
-      <c r="BG3" s="95"/>
-      <c r="BH3" s="95"/>
-      <c r="BI3" s="96"/>
-      <c r="BJ3" s="96"/>
-      <c r="BK3" s="96"/>
-      <c r="BL3" s="96"/>
-      <c r="BM3" s="96"/>
-      <c r="BN3" s="96"/>
-      <c r="BO3" s="96"/>
-      <c r="BP3" s="96"/>
-      <c r="BQ3" s="96"/>
-      <c r="BR3" s="97"/>
-      <c r="BS3" s="97"/>
-      <c r="BT3" s="97"/>
-      <c r="BU3" s="97"/>
-      <c r="BV3" s="97"/>
-      <c r="BW3" s="97"/>
-      <c r="BX3" s="90"/>
-      <c r="BY3" s="90"/>
-      <c r="BZ3" s="90"/>
-      <c r="CA3" s="90"/>
-      <c r="CB3" s="90"/>
-      <c r="CC3" s="90"/>
-      <c r="CD3" s="90"/>
-      <c r="CE3" s="90"/>
-      <c r="CF3" s="90"/>
-      <c r="CG3" s="90"/>
-      <c r="CH3" s="90"/>
-      <c r="CI3" s="90"/>
-    </row>
-    <row r="4" spans="1:87" s="11" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="77" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="79" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="79" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="79" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="79" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="81" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>12</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="10">
@@ -1948,445 +2035,445 @@
       </c>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
-      <c r="M4" s="70">
+      <c r="M4" s="69">
         <v>2</v>
       </c>
-      <c r="N4" s="70"/>
-      <c r="O4" s="70"/>
-      <c r="P4" s="70"/>
-      <c r="Q4" s="70"/>
-      <c r="R4" s="70">
+      <c r="N4" s="69"/>
+      <c r="O4" s="69"/>
+      <c r="P4" s="69"/>
+      <c r="Q4" s="69"/>
+      <c r="R4" s="69">
         <v>3</v>
       </c>
-      <c r="S4" s="70"/>
-      <c r="T4" s="70"/>
-      <c r="U4" s="70"/>
-      <c r="V4" s="70"/>
-      <c r="W4" s="70">
+      <c r="S4" s="69"/>
+      <c r="T4" s="69"/>
+      <c r="U4" s="69"/>
+      <c r="V4" s="69"/>
+      <c r="W4" s="69">
         <v>4</v>
       </c>
-      <c r="X4" s="70"/>
-      <c r="Y4" s="70"/>
-      <c r="Z4" s="70"/>
-      <c r="AA4" s="70"/>
-      <c r="AB4" s="70">
+      <c r="X4" s="69"/>
+      <c r="Y4" s="69"/>
+      <c r="Z4" s="69"/>
+      <c r="AA4" s="69"/>
+      <c r="AB4" s="69">
         <v>5</v>
       </c>
-      <c r="AC4" s="70"/>
-      <c r="AD4" s="70"/>
-      <c r="AE4" s="70"/>
-      <c r="AF4" s="70"/>
-      <c r="AG4" s="70">
+      <c r="AC4" s="69"/>
+      <c r="AD4" s="69"/>
+      <c r="AE4" s="69"/>
+      <c r="AF4" s="69"/>
+      <c r="AG4" s="69">
         <v>6</v>
       </c>
-      <c r="AH4" s="70"/>
-      <c r="AI4" s="70"/>
-      <c r="AJ4" s="70"/>
-      <c r="AK4" s="70"/>
-      <c r="AL4" s="70">
+      <c r="AH4" s="69"/>
+      <c r="AI4" s="69"/>
+      <c r="AJ4" s="69"/>
+      <c r="AK4" s="69"/>
+      <c r="AL4" s="69">
         <v>7</v>
       </c>
-      <c r="AM4" s="70"/>
-      <c r="AN4" s="70"/>
-      <c r="AO4" s="70"/>
-      <c r="AP4" s="70"/>
-      <c r="AQ4" s="73">
+      <c r="AM4" s="69"/>
+      <c r="AN4" s="69"/>
+      <c r="AO4" s="69"/>
+      <c r="AP4" s="69"/>
+      <c r="AQ4" s="87">
         <v>8</v>
       </c>
-      <c r="AR4" s="73"/>
-      <c r="AS4" s="73"/>
-      <c r="AT4" s="73"/>
-      <c r="AU4" s="73"/>
-      <c r="AV4" s="70">
+      <c r="AR4" s="87"/>
+      <c r="AS4" s="87"/>
+      <c r="AT4" s="87"/>
+      <c r="AU4" s="87"/>
+      <c r="AV4" s="69">
         <v>9</v>
       </c>
-      <c r="AW4" s="70"/>
-      <c r="AX4" s="70"/>
-      <c r="AY4" s="70"/>
-      <c r="AZ4" s="70"/>
-      <c r="BA4" s="70">
+      <c r="AW4" s="69"/>
+      <c r="AX4" s="69"/>
+      <c r="AY4" s="69"/>
+      <c r="AZ4" s="69"/>
+      <c r="BA4" s="69">
         <v>10</v>
       </c>
-      <c r="BB4" s="70"/>
-      <c r="BC4" s="70"/>
-      <c r="BD4" s="70"/>
-      <c r="BE4" s="70"/>
-      <c r="BF4" s="70">
+      <c r="BB4" s="69"/>
+      <c r="BC4" s="69"/>
+      <c r="BD4" s="69"/>
+      <c r="BE4" s="69"/>
+      <c r="BF4" s="69">
         <v>11</v>
       </c>
-      <c r="BG4" s="70"/>
-      <c r="BH4" s="70"/>
-      <c r="BI4" s="70"/>
-      <c r="BJ4" s="70"/>
-      <c r="BK4" s="71">
+      <c r="BG4" s="69"/>
+      <c r="BH4" s="69"/>
+      <c r="BI4" s="69"/>
+      <c r="BJ4" s="69"/>
+      <c r="BK4" s="88">
         <v>12</v>
       </c>
-      <c r="BL4" s="72"/>
-      <c r="BM4" s="72"/>
-      <c r="BN4" s="72"/>
-      <c r="BO4" s="72"/>
-      <c r="BP4" s="70">
+      <c r="BL4" s="89"/>
+      <c r="BM4" s="89"/>
+      <c r="BN4" s="89"/>
+      <c r="BO4" s="89"/>
+      <c r="BP4" s="69">
         <v>13</v>
       </c>
-      <c r="BQ4" s="70"/>
-      <c r="BR4" s="70"/>
-      <c r="BS4" s="70"/>
-      <c r="BT4" s="70"/>
-      <c r="BU4" s="70">
+      <c r="BQ4" s="69"/>
+      <c r="BR4" s="69"/>
+      <c r="BS4" s="69"/>
+      <c r="BT4" s="69"/>
+      <c r="BU4" s="69">
         <v>15</v>
       </c>
-      <c r="BV4" s="70"/>
-      <c r="BW4" s="70"/>
-      <c r="BX4" s="70"/>
-      <c r="BY4" s="70">
+      <c r="BV4" s="69"/>
+      <c r="BW4" s="69"/>
+      <c r="BX4" s="69"/>
+      <c r="BY4" s="69">
         <v>16</v>
       </c>
-      <c r="BZ4" s="70"/>
-      <c r="CA4" s="70"/>
-      <c r="CB4" s="70"/>
-      <c r="CC4" s="70"/>
-      <c r="CD4" s="70">
+      <c r="BZ4" s="69"/>
+      <c r="CA4" s="69"/>
+      <c r="CB4" s="69"/>
+      <c r="CC4" s="69"/>
+      <c r="CD4" s="69">
         <v>17</v>
       </c>
-      <c r="CE4" s="70"/>
-      <c r="CF4" s="70"/>
-      <c r="CG4" s="70"/>
-      <c r="CH4" s="70"/>
-    </row>
-    <row r="5" spans="1:87" s="11" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="77"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="52">
+      <c r="CE4" s="69"/>
+      <c r="CF4" s="69"/>
+      <c r="CG4" s="69"/>
+      <c r="CH4" s="69"/>
+    </row>
+    <row r="5" spans="1:87" s="11" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="73"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="49">
         <v>44250</v>
       </c>
-      <c r="I5" s="53">
+      <c r="I5" s="98">
         <f>H5+1</f>
         <v>44251</v>
       </c>
-      <c r="J5" s="53">
+      <c r="J5" s="98">
         <f t="shared" ref="J5:X5" si="0">I5+1</f>
         <v>44252</v>
       </c>
-      <c r="K5" s="53">
+      <c r="K5" s="98">
         <f t="shared" si="0"/>
         <v>44253</v>
       </c>
-      <c r="L5" s="53">
+      <c r="L5" s="98">
         <f t="shared" si="0"/>
         <v>44254</v>
       </c>
-      <c r="M5" s="53">
+      <c r="M5" s="98">
         <f t="shared" si="0"/>
         <v>44255</v>
       </c>
-      <c r="N5" s="53">
+      <c r="N5" s="98">
         <f t="shared" si="0"/>
         <v>44256</v>
       </c>
-      <c r="O5" s="53">
+      <c r="O5" s="98">
         <f t="shared" si="0"/>
         <v>44257</v>
       </c>
-      <c r="P5" s="53">
+      <c r="P5" s="98">
         <f t="shared" si="0"/>
         <v>44258</v>
       </c>
-      <c r="Q5" s="53">
+      <c r="Q5" s="97">
         <f t="shared" si="0"/>
         <v>44259</v>
       </c>
-      <c r="R5" s="53">
+      <c r="R5" s="97">
         <f t="shared" si="0"/>
         <v>44260</v>
       </c>
-      <c r="S5" s="53">
+      <c r="S5" s="97">
         <f t="shared" si="0"/>
         <v>44261</v>
       </c>
-      <c r="T5" s="53">
+      <c r="T5" s="97">
         <f t="shared" si="0"/>
         <v>44262</v>
       </c>
-      <c r="U5" s="53">
+      <c r="U5" s="97">
         <f t="shared" si="0"/>
         <v>44263</v>
       </c>
-      <c r="V5" s="53">
+      <c r="V5" s="97">
         <f t="shared" si="0"/>
         <v>44264</v>
       </c>
-      <c r="W5" s="53">
+      <c r="W5" s="97">
         <f t="shared" si="0"/>
         <v>44265</v>
       </c>
-      <c r="X5" s="53">
+      <c r="X5" s="97">
         <f t="shared" si="0"/>
         <v>44266</v>
       </c>
-      <c r="Y5" s="54">
+      <c r="Y5" s="97">
         <f t="shared" ref="Y5" si="1">X5+1</f>
         <v>44267</v>
       </c>
-      <c r="Z5" s="54">
+      <c r="Z5" s="97">
         <f t="shared" ref="Z5" si="2">Y5+1</f>
         <v>44268</v>
       </c>
-      <c r="AA5" s="54">
+      <c r="AA5" s="97">
         <f t="shared" ref="AA5" si="3">Z5+1</f>
         <v>44269</v>
       </c>
-      <c r="AB5" s="54">
+      <c r="AB5" s="97">
         <f t="shared" ref="AB5" si="4">AA5+1</f>
         <v>44270</v>
       </c>
-      <c r="AC5" s="54">
+      <c r="AC5" s="97">
         <f t="shared" ref="AC5" si="5">AB5+1</f>
         <v>44271</v>
       </c>
-      <c r="AD5" s="54">
+      <c r="AD5" s="97">
         <f t="shared" ref="AD5" si="6">AC5+1</f>
         <v>44272</v>
       </c>
-      <c r="AE5" s="54">
+      <c r="AE5" s="97">
         <f t="shared" ref="AE5" si="7">AD5+1</f>
         <v>44273</v>
       </c>
-      <c r="AF5" s="54">
+      <c r="AF5" s="96">
         <f t="shared" ref="AF5" si="8">AE5+1</f>
         <v>44274</v>
       </c>
-      <c r="AG5" s="54">
+      <c r="AG5" s="96">
         <f t="shared" ref="AG5" si="9">AF5+1</f>
         <v>44275</v>
       </c>
-      <c r="AH5" s="54">
+      <c r="AH5" s="96">
         <f t="shared" ref="AH5" si="10">AG5+1</f>
         <v>44276</v>
       </c>
-      <c r="AI5" s="55">
+      <c r="AI5" s="96">
         <f t="shared" ref="AI5" si="11">AH5+1</f>
         <v>44277</v>
       </c>
-      <c r="AJ5" s="55">
+      <c r="AJ5" s="96">
         <f t="shared" ref="AJ5" si="12">AI5+1</f>
         <v>44278</v>
       </c>
-      <c r="AK5" s="55">
+      <c r="AK5" s="96">
         <f t="shared" ref="AK5" si="13">AJ5+1</f>
         <v>44279</v>
       </c>
-      <c r="AL5" s="55">
+      <c r="AL5" s="96">
         <f t="shared" ref="AL5" si="14">AK5+1</f>
         <v>44280</v>
       </c>
-      <c r="AM5" s="55">
+      <c r="AM5" s="96">
         <f t="shared" ref="AM5" si="15">AL5+1</f>
         <v>44281</v>
       </c>
-      <c r="AN5" s="55">
+      <c r="AN5" s="96">
         <f t="shared" ref="AN5" si="16">AM5+1</f>
         <v>44282</v>
       </c>
-      <c r="AO5" s="55">
+      <c r="AO5" s="96">
         <f t="shared" ref="AO5" si="17">AN5+1</f>
         <v>44283</v>
       </c>
-      <c r="AP5" s="55">
+      <c r="AP5" s="96">
         <f t="shared" ref="AP5" si="18">AO5+1</f>
         <v>44284</v>
       </c>
-      <c r="AQ5" s="55">
+      <c r="AQ5" s="96">
         <f t="shared" ref="AQ5" si="19">AP5+1</f>
         <v>44285</v>
       </c>
-      <c r="AR5" s="55">
+      <c r="AR5" s="96">
         <f t="shared" ref="AR5" si="20">AQ5+1</f>
         <v>44286</v>
       </c>
-      <c r="AS5" s="55">
+      <c r="AS5" s="96">
         <f t="shared" ref="AS5" si="21">AR5+1</f>
         <v>44287</v>
       </c>
-      <c r="AT5" s="55">
+      <c r="AT5" s="96">
         <f t="shared" ref="AT5" si="22">AS5+1</f>
         <v>44288</v>
       </c>
-      <c r="AU5" s="55">
+      <c r="AU5" s="96">
         <f t="shared" ref="AU5" si="23">AT5+1</f>
         <v>44289</v>
       </c>
-      <c r="AV5" s="55">
+      <c r="AV5" s="96">
         <f t="shared" ref="AV5" si="24">AU5+1</f>
         <v>44290</v>
       </c>
-      <c r="AW5" s="55">
+      <c r="AW5" s="96">
         <f t="shared" ref="AW5" si="25">AV5+1</f>
         <v>44291</v>
       </c>
-      <c r="AX5" s="55">
+      <c r="AX5" s="96">
         <f t="shared" ref="AX5" si="26">AW5+1</f>
         <v>44292</v>
       </c>
-      <c r="AY5" s="55">
+      <c r="AY5" s="96">
         <f t="shared" ref="AY5" si="27">AX5+1</f>
         <v>44293</v>
       </c>
-      <c r="AZ5" s="55">
+      <c r="AZ5" s="96">
         <f t="shared" ref="AZ5" si="28">AY5+1</f>
         <v>44294</v>
       </c>
-      <c r="BA5" s="55">
+      <c r="BA5" s="96">
         <f t="shared" ref="BA5" si="29">AZ5+1</f>
         <v>44295</v>
       </c>
-      <c r="BB5" s="55">
+      <c r="BB5" s="96">
         <f t="shared" ref="BB5" si="30">BA5+1</f>
         <v>44296</v>
       </c>
-      <c r="BC5" s="55">
+      <c r="BC5" s="96">
         <f t="shared" ref="BC5" si="31">BB5+1</f>
         <v>44297</v>
       </c>
-      <c r="BD5" s="55">
+      <c r="BD5" s="96">
         <f t="shared" ref="BD5" si="32">BC5+1</f>
         <v>44298</v>
       </c>
-      <c r="BE5" s="55">
+      <c r="BE5" s="96">
         <f t="shared" ref="BE5" si="33">BD5+1</f>
         <v>44299</v>
       </c>
-      <c r="BF5" s="55">
+      <c r="BF5" s="96">
         <f t="shared" ref="BF5" si="34">BE5+1</f>
         <v>44300</v>
       </c>
-      <c r="BG5" s="55">
+      <c r="BG5" s="96">
         <f t="shared" ref="BG5" si="35">BF5+1</f>
         <v>44301</v>
       </c>
-      <c r="BH5" s="55">
+      <c r="BH5" s="96">
         <f t="shared" ref="BH5" si="36">BG5+1</f>
         <v>44302</v>
       </c>
-      <c r="BI5" s="56">
+      <c r="BI5" s="50">
         <f t="shared" ref="BI5" si="37">BH5+1</f>
         <v>44303</v>
       </c>
-      <c r="BJ5" s="56">
+      <c r="BJ5" s="50">
         <f t="shared" ref="BJ5" si="38">BI5+1</f>
         <v>44304</v>
       </c>
-      <c r="BK5" s="56">
+      <c r="BK5" s="50">
         <f t="shared" ref="BK5" si="39">BJ5+1</f>
         <v>44305</v>
       </c>
-      <c r="BL5" s="56">
+      <c r="BL5" s="50">
         <f t="shared" ref="BL5" si="40">BK5+1</f>
         <v>44306</v>
       </c>
-      <c r="BM5" s="56">
+      <c r="BM5" s="50">
         <f t="shared" ref="BM5" si="41">BL5+1</f>
         <v>44307</v>
       </c>
-      <c r="BN5" s="56">
+      <c r="BN5" s="50">
         <f t="shared" ref="BN5" si="42">BM5+1</f>
         <v>44308</v>
       </c>
-      <c r="BO5" s="56">
+      <c r="BO5" s="50">
         <f t="shared" ref="BO5" si="43">BN5+1</f>
         <v>44309</v>
       </c>
-      <c r="BP5" s="56">
+      <c r="BP5" s="50">
         <f t="shared" ref="BP5" si="44">BO5+1</f>
         <v>44310</v>
       </c>
-      <c r="BQ5" s="56">
+      <c r="BQ5" s="50">
         <f t="shared" ref="BQ5" si="45">BP5+1</f>
         <v>44311</v>
       </c>
-      <c r="BR5" s="57">
+      <c r="BR5" s="51">
         <f t="shared" ref="BR5" si="46">BQ5+1</f>
         <v>44312</v>
       </c>
-      <c r="BS5" s="57">
+      <c r="BS5" s="51">
         <f t="shared" ref="BS5" si="47">BR5+1</f>
         <v>44313</v>
       </c>
-      <c r="BT5" s="57">
+      <c r="BT5" s="51">
         <f t="shared" ref="BT5" si="48">BS5+1</f>
         <v>44314</v>
       </c>
-      <c r="BU5" s="57">
+      <c r="BU5" s="51">
         <f t="shared" ref="BU5" si="49">BT5+1</f>
         <v>44315</v>
       </c>
-      <c r="BV5" s="57">
+      <c r="BV5" s="51">
         <f t="shared" ref="BV5" si="50">BU5+1</f>
         <v>44316</v>
       </c>
-      <c r="BW5" s="57">
+      <c r="BW5" s="51">
         <f t="shared" ref="BW5" si="51">BV5+1</f>
         <v>44317</v>
       </c>
-      <c r="BX5" s="52">
+      <c r="BX5" s="48">
         <f t="shared" ref="BX5" si="52">BW5+1</f>
         <v>44318</v>
       </c>
-      <c r="BY5" s="52">
+      <c r="BY5" s="48">
         <f t="shared" ref="BY5" si="53">BX5+1</f>
         <v>44319</v>
       </c>
-      <c r="BZ5" s="52">
+      <c r="BZ5" s="48">
         <f t="shared" ref="BZ5" si="54">BY5+1</f>
         <v>44320</v>
       </c>
-      <c r="CA5" s="52">
+      <c r="CA5" s="48">
         <f t="shared" ref="CA5" si="55">BZ5+1</f>
         <v>44321</v>
       </c>
-      <c r="CB5" s="52">
+      <c r="CB5" s="48">
         <f t="shared" ref="CB5" si="56">CA5+1</f>
         <v>44322</v>
       </c>
-      <c r="CC5" s="52">
+      <c r="CC5" s="48">
         <f t="shared" ref="CC5" si="57">CB5+1</f>
         <v>44323</v>
       </c>
-      <c r="CD5" s="52">
+      <c r="CD5" s="48">
         <f t="shared" ref="CD5" si="58">CC5+1</f>
         <v>44324</v>
       </c>
-      <c r="CE5" s="52">
+      <c r="CE5" s="48">
         <f t="shared" ref="CE5" si="59">CD5+1</f>
         <v>44325</v>
       </c>
-      <c r="CF5" s="52">
+      <c r="CF5" s="48">
         <f t="shared" ref="CF5" si="60">CE5+1</f>
         <v>44326</v>
       </c>
-      <c r="CG5" s="52">
+      <c r="CG5" s="48">
         <f t="shared" ref="CG5" si="61">CF5+1</f>
         <v>44327</v>
       </c>
-      <c r="CH5" s="52">
+      <c r="CH5" s="48">
         <f t="shared" ref="CH5" si="62">CG5+1</f>
         <v>44328</v>
       </c>
-      <c r="CI5" s="52">
+      <c r="CI5" s="48">
         <f t="shared" ref="CI5" si="63">CH5+1</f>
         <v>44329</v>
       </c>
     </row>
     <row r="6" spans="1:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="78"/>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="80"/>
-      <c r="G6" s="80"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
       <c r="H6" s="3">
         <v>1</v>
       </c>
@@ -2629,33 +2716,33 @@
       </c>
     </row>
     <row r="7" spans="1:87" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="62">
+      <c r="C7" s="56">
         <v>1</v>
       </c>
-      <c r="D7" s="62">
-        <v>16</v>
-      </c>
-      <c r="E7" s="62">
+      <c r="D7" s="56">
         <v>1</v>
       </c>
-      <c r="F7" s="62">
-        <v>0</v>
-      </c>
-      <c r="G7" s="63">
+      <c r="E7" s="56">
+        <v>1</v>
+      </c>
+      <c r="F7" s="56">
+        <v>0</v>
+      </c>
+      <c r="G7" s="57">
         <f>(G8+G9+G10)/4</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:87" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29"/>
+      <c r="A8" s="67"/>
       <c r="B8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="7">
         <v>1</v>
@@ -2674,15 +2761,15 @@
       </c>
     </row>
     <row r="9" spans="1:87" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="29"/>
+      <c r="A9" s="67"/>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="7">
         <v>1</v>
       </c>
       <c r="D9" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="7">
         <v>1</v>
@@ -2693,15 +2780,15 @@
       </c>
     </row>
     <row r="10" spans="1:87" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="29"/>
+      <c r="A10" s="67"/>
       <c r="B10" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="7">
         <v>1</v>
       </c>
       <c r="D10" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" s="7">
         <v>1</v>
@@ -2712,28 +2799,36 @@
       </c>
     </row>
     <row r="11" spans="1:87" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
-        <v>13</v>
+      <c r="A11" s="66" t="s">
+        <v>12</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="68"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="68"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="69">
-        <f>SUM(G12:G18)/7</f>
+        <v>12</v>
+      </c>
+      <c r="C11" s="60">
+        <v>2</v>
+      </c>
+      <c r="D11" s="60">
+        <v>8</v>
+      </c>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="61">
+        <f>SUM(G12:G15)/7</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:87" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22"/>
+      <c r="A12" s="66"/>
       <c r="B12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="C12" s="7">
+        <v>1</v>
+      </c>
+      <c r="D12" s="7">
+        <v>15</v>
+      </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="8">
@@ -2741,11 +2836,13 @@
       </c>
     </row>
     <row r="13" spans="1:87" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22"/>
+      <c r="A13" s="66"/>
       <c r="B13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="7"/>
+        <v>20</v>
+      </c>
+      <c r="C13" s="7">
+        <v>1</v>
+      </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -2754,12 +2851,16 @@
       </c>
     </row>
     <row r="14" spans="1:87" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
+      <c r="A14" s="66"/>
       <c r="B14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+        <v>21</v>
+      </c>
+      <c r="C14" s="7">
+        <v>6</v>
+      </c>
+      <c r="D14" s="7">
+        <v>4</v>
+      </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="8">
@@ -2767,35 +2868,39 @@
       </c>
     </row>
     <row r="15" spans="1:87" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22"/>
-      <c r="B15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
+      <c r="A15" s="66"/>
+      <c r="B15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="7">
+        <v>11</v>
+      </c>
+      <c r="D15" s="7">
+        <v>1</v>
+      </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:87" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="22"/>
-      <c r="B16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8">
-        <v>0</v>
-      </c>
+    <row r="16" spans="1:87" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="22"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="6" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -2806,12 +2911,16 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+        <v>37</v>
+      </c>
+      <c r="C18" s="7">
+        <v>10</v>
+      </c>
+      <c r="D18" s="7">
+        <v>5</v>
+      </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="8">
@@ -2819,28 +2928,36 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="24"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8"/>
+      <c r="A19" s="62"/>
+      <c r="B19" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="64">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="24"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8">
+      <c r="A20" s="62"/>
+      <c r="B20" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="64">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="24"/>
-      <c r="B21" s="23"/>
+      <c r="A21" s="62"/>
+      <c r="B21" s="58" t="s">
+        <v>40</v>
+      </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
@@ -2850,19 +2967,23 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="34"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33">
+      <c r="A22" s="62"/>
+      <c r="B22" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="66"/>
-      <c r="B23" s="64"/>
+      <c r="A23" s="62"/>
+      <c r="B23" s="58" t="s">
+        <v>42</v>
+      </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
@@ -2872,8 +2993,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="65"/>
-      <c r="B24" s="64"/>
+      <c r="A24" s="62"/>
+      <c r="B24" s="58" t="s">
+        <v>43</v>
+      </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
@@ -2882,31 +3005,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="65"/>
-      <c r="B25" s="64"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="8">
+    <row r="25" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="62"/>
+      <c r="B25" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="63"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="63"/>
+      <c r="G25" s="64">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="65"/>
-      <c r="B26" s="64"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="65"/>
-      <c r="B27" s="64"/>
+      <c r="A26" s="62"/>
+      <c r="B26" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="62"/>
+      <c r="B27" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
@@ -2916,19 +3045,19 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="65"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="25"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="25"/>
-      <c r="B29" s="23"/>
+      <c r="B29" s="6"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
@@ -2938,19 +3067,19 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="27"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="27"/>
-      <c r="B31" s="23"/>
+      <c r="A30" s="31"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="59"/>
+      <c r="B31" s="6"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
@@ -2959,8 +3088,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="27"/>
+    <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="24"/>
       <c r="B32" s="6"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -2970,19 +3099,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="35"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="67"/>
+    <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="24"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="24"/>
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -2993,19 +3122,18 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="26"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="8">
+      <c r="A35" s="32"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="26"/>
-      <c r="B36" s="6"/>
+      <c r="A36" s="34"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
@@ -3015,51 +3143,73 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="26"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="36"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="38"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="37"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="33">
-        <v>0</v>
-      </c>
+      <c r="A37" s="33"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="7">
+        <v>0</v>
+      </c>
+      <c r="D38" s="7">
+        <v>0</v>
+      </c>
+      <c r="E38" s="7">
+        <v>0</v>
+      </c>
+      <c r="F38" s="7">
+        <v>0</v>
+      </c>
+      <c r="G38" s="8"/>
+    </row>
+    <row r="39" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="7">
+        <v>0</v>
+      </c>
+      <c r="D39" s="7">
+        <v>0</v>
+      </c>
+      <c r="E39" s="7">
+        <v>0</v>
+      </c>
+      <c r="F39" s="7">
+        <v>0</v>
+      </c>
+      <c r="G39" s="8"/>
+    </row>
+    <row r="40" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="7">
+        <v>0</v>
+      </c>
+      <c r="D40" s="7">
+        <v>0</v>
+      </c>
+      <c r="E40" s="7">
+        <v>0</v>
+      </c>
+      <c r="F40" s="7">
+        <v>0</v>
+      </c>
+      <c r="G40" s="8"/>
     </row>
     <row r="41" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C41" s="7">
         <v>0</v>
@@ -3075,69 +3225,11 @@
       </c>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" s="7">
-        <v>0</v>
-      </c>
-      <c r="D42" s="7">
-        <v>0</v>
-      </c>
-      <c r="E42" s="7">
-        <v>0</v>
-      </c>
-      <c r="F42" s="7">
-        <v>0</v>
-      </c>
-      <c r="G42" s="8"/>
-    </row>
-    <row r="43" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" s="7">
-        <v>0</v>
-      </c>
-      <c r="D43" s="7">
-        <v>0</v>
-      </c>
-      <c r="E43" s="7">
-        <v>0</v>
-      </c>
-      <c r="F43" s="7">
-        <v>0</v>
-      </c>
-      <c r="G43" s="8"/>
-    </row>
-    <row r="44" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" s="7">
-        <v>0</v>
-      </c>
-      <c r="D44" s="7">
-        <v>0</v>
-      </c>
-      <c r="E44" s="7">
-        <v>0</v>
-      </c>
-      <c r="F44" s="7">
-        <v>0</v>
-      </c>
-      <c r="G44" s="8"/>
-    </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="BX3:CI3"/>
-    <mergeCell ref="I3:X3"/>
-    <mergeCell ref="Y3:AH3"/>
-    <mergeCell ref="AI3:BH3"/>
-    <mergeCell ref="BI3:BQ3"/>
-    <mergeCell ref="BR3:BW3"/>
-    <mergeCell ref="CD4:CH4"/>
+  <mergeCells count="30">
+    <mergeCell ref="BF4:BJ4"/>
+    <mergeCell ref="BK4:BO4"/>
+    <mergeCell ref="BP4:BT4"/>
     <mergeCell ref="AI2:AP2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B4:B6"/>
@@ -3154,6 +3246,10 @@
     <mergeCell ref="R4:V4"/>
     <mergeCell ref="W4:AA4"/>
     <mergeCell ref="AB4:AF4"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="I3:X3"/>
+    <mergeCell ref="CD4:CH4"/>
     <mergeCell ref="AG4:AK4"/>
     <mergeCell ref="AL4:AP4"/>
     <mergeCell ref="AQ4:AU4"/>
@@ -3161,11 +3257,8 @@
     <mergeCell ref="BA4:BE4"/>
     <mergeCell ref="BU4:BX4"/>
     <mergeCell ref="BY4:CC4"/>
-    <mergeCell ref="BF4:BJ4"/>
-    <mergeCell ref="BK4:BO4"/>
-    <mergeCell ref="BP4:BT4"/>
   </mergeCells>
-  <conditionalFormatting sqref="H29:CF44 H7:CF27">
+  <conditionalFormatting sqref="H26:CF41 H7:CF24">
     <cfRule type="expression" dxfId="17" priority="9">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -3191,7 +3284,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B45:BO45">
+  <conditionalFormatting sqref="B42:BO42">
     <cfRule type="expression" dxfId="9" priority="10">
       <formula>TRUE</formula>
     </cfRule>
@@ -3201,7 +3294,7 @@
       <formula>H$6=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H28:CF28">
+  <conditionalFormatting sqref="H25:CF25">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -3227,8 +3320,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="16">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+  <dataValidations count="15">
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2:H3" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
@@ -3244,7 +3336,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E4:E6" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F4:F6" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G4:G6" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="C1" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F3" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
@@ -3253,7 +3345,8 @@
   <headerFooter differentFirst="1">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3273,113 +3366,113 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="39"/>
-    <col min="2" max="3" width="12.5" style="39" customWidth="1"/>
-    <col min="4" max="4" width="19.375" style="39" customWidth="1"/>
-    <col min="5" max="5" width="56.875" style="39" customWidth="1"/>
-    <col min="6" max="16384" width="8.875" style="39"/>
+    <col min="1" max="1" width="8.875" style="35"/>
+    <col min="2" max="3" width="12.5" style="35" customWidth="1"/>
+    <col min="4" max="4" width="19.375" style="35" customWidth="1"/>
+    <col min="5" max="5" width="56.875" style="35" customWidth="1"/>
+    <col min="6" max="16384" width="8.875" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="51" t="s">
-        <v>9</v>
+    <row r="1" spans="2:5" s="46" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="47" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="D4" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="43" t="s">
+      <c r="E4" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="44" t="s">
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="41">
+        <v>0</v>
+      </c>
+      <c r="C5" s="37">
+        <v>43487</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="42" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="45">
-        <v>0</v>
-      </c>
-      <c r="C5" s="41">
-        <v>43487</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="46" t="s">
-        <v>8</v>
-      </c>
-    </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="45"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="46"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="42"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="45"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="46"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="42"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="45"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="46"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="42"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="45"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="46"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="42"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="45"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="46"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="42"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="45"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="46"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="42"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="45"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="46"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="42"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="45"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="46"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="42"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="45"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="46"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="42"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="45"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="46"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="42"/>
     </row>
     <row r="16" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="47"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="49"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3387,21 +3480,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CD84185944F91A458BABF3F84844BC85" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d7aae08a9dea3742d61b8098d05448f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ce0a8dfd-918e-473b-8ccc-59cfa4cbf1af" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="13f737887d6b3d8ad10810ec5113674c" ns2:_="">
     <xsd:import namespace="ce0a8dfd-918e-473b-8ccc-59cfa4cbf1af"/>
@@ -3533,10 +3611,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3CDDCE5-7EB7-43D6-82FE-E5EFC3D759BE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D200AD4B-7A33-4A60-992C-3323A4EEF5D2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ce0a8dfd-918e-473b-8ccc-59cfa4cbf1af"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3558,19 +3661,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D200AD4B-7A33-4A60-992C-3323A4EEF5D2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3CDDCE5-7EB7-43D6-82FE-E5EFC3D759BE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ce0a8dfd-918e-473b-8ccc-59cfa4cbf1af"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>